<commit_message>
🤖 Publica dados no site (31/10/2025 10:41)
</commit_message>
<xml_diff>
--- a/site/downloads/concorrencia_2026.xlsx
+++ b/site/downloads/concorrencia_2026.xlsx
@@ -21,7 +21,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNIFESP" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNICAMP" sheetId="13" state="visible" r:id="rId13"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instituto do Câncer do Ceará – " sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UFPA" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5928,6 +5929,377 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>PROGRAMA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>VAGAS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>INSCRITOS</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CONCORRÊNCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Clínica Médica (Belém)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Clínica Médica (Altamira)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cirurgia Geral (Belém)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>169</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>28,17</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Dermatologia (Belém)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>23,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ginecologia e Obstetrícia (Belém)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>15,83</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Medicina de Família e Comunidade (Belém)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>13,3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Medicina de Família e Comunidade (Altamira)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Oftalmologia (Belém)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Otorrinolaringologia (Belém)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>22,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Pediatria (Belém)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>11,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Endocrinologia (Belém)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Geriatria (Belém)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Oncologia Clínica (Belém)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Pneumologia (Belém)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Medicina Paliativa (Belém)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
🤖 Publica dados no site (01/11/2025 10:35)
</commit_message>
<xml_diff>
--- a/site/downloads/concorrencia_2026.xlsx
+++ b/site/downloads/concorrencia_2026.xlsx
@@ -13,16 +13,17 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SMS-Curitiba" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UFCSPA" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UEL" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HIAE" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HOS BOS" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Santa Casa de Limeira" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SES-RJ" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UERJ" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNIFESP" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNICAMP" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instituto do Câncer do Ceará – " sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UFPA" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNESP" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HIAE" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HOS BOS" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Santa Casa de Limeira" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SES-RJ" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UERJ" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNIFESP" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNICAMP" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instituto do Câncer do Ceará – " sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UFPA" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2511,6 +2512,443 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>PROGRAMA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>VAGAS TOTAIS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>INSCRITOS</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CONCORRÊNCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Anestesiologia</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Angiorradiologia e Cirurgia Endovascular</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cardiologia</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cirurgia Cardiovascular</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cirurgia Geral</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>196</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cirurgia Vascular</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>4,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Clínica Médica</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>166</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>41,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ginecologia e Obstetrícia</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>216</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>43,2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Medicina de Família e Comunidade</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>7,67</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Medicina Intensiva Pediátrica</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Neonatologia</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Neurocirurgia</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Oftalmologia</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>48,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Oncologia Clínica</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Ortopedia e Traumatologia</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>31,75</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Otorrinolaringologia</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Pediatria</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>157</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>39,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Urologia</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4252,7 +4690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4450,619 +4888,6 @@
       <c r="C11" t="inlineStr">
         <is>
           <t>40,5</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>PROGRAMA</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL VAGAS</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL INSCRITOS</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>CONCORRÊNCIA GERAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Acupuntura</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>5,3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Anestesiologia</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>339</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>33,9</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Cirurgia Cardiovascular</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Cirurgia Geral</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>704</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Clínica Médica</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>905</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>17,4</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Dermatologia</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>370</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>46,3</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Genética Médica</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>17,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Infectologia</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Medicina de Emergência</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>5,8</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Medicina de Família e Comunidade</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>8,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Medicina de Tráfego</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0,7</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Medicina Esportiva</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>142</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>28,4</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Medicina Intensiva</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>5,6</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Medicina Preventiva e Social</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Neurocirurgia</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>204</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Neurologia</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>37,1</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Obstetrícia e Ginecologia</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>454</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>37,8</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Oftalmologia</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>443</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>36,9</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Ortopedia e Traumatologia</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>319</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>19,9</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Otorrinolaringologia</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>43,3</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Patologia</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>15,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Patologia Clínica e Medicina Laboratorial</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Pediatria</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>310</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>17,2</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Psiquiatria</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>552</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>36,8</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Radiologia e Diagnóstico por Imagem</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>232</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>19,3</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Radioterapia</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
     </row>
@@ -5088,139 +4913,139 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PROGRAMAS ACESSO DIRETO</t>
+          <t>PROGRAMA</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>CANDIDATOS</t>
+          <t>TOTAL VAGAS</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>VAGAS DISPONÍVEIS</t>
+          <t>TOTAL INSCRITOS</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CONCORRÊNCIA</t>
+          <t>CONCORRÊNCIA GERAL</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ANESTESIOLOGIA</t>
+          <t>Acupuntura</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>16</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>24,10</t>
+          <t>5,3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CIRURGIA CARDIOVASCULAR</t>
+          <t>Anestesiologia</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>339</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>18,00</t>
+          <t>33,9</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CIRURGIA GERAL</t>
+          <t>Cirurgia Cardiovascular</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>483</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>36</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>40,25</t>
+          <t>18</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CLINICA MEDICA</t>
+          <t>Cirurgia Geral</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>575</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>704</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>15,54</t>
+          <t>44</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DERMATOLOGIA</t>
+          <t>Clínica Médica</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>52</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>905</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>48,80</t>
+          <t>17,4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DERMATOLOGIA – COMPROMISSO SOCIAL</t>
+          <t>Dermatologia</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -5230,452 +5055,452 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>370</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>46,3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GENETICA MEDICA</t>
+          <t>Genética Médica</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>17,5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>INFECTOLOGIA</t>
+          <t>Infectologia</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>42</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>7,80</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MEDICINA DE EMERGENCIA</t>
+          <t>Medicina de Emergência</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>64</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4,75</t>
+          <t>5,8</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MEDICINA DE FAMILIA E COMUNIDADE</t>
+          <t>Medicina de Família e Comunidade</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>34</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>10,07</t>
+          <t>8,5</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MEDICINA DO TRABALHO</t>
+          <t>Medicina de Tráfego</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>7,25</t>
+          <t>0,7</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MEDICINA INTENSIVA</t>
+          <t>Medicina Esportiva</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>142</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5,71</t>
+          <t>28,4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MEDICINA NUCLEAR</t>
+          <t>Medicina Intensiva</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>56</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>8,33</t>
+          <t>5,6</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MEDICINA PREVENTIVA E SOCIAL</t>
+          <t>Medicina Preventiva e Social</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1,25</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>NEUROCIRURGIA</t>
+          <t>Neurocirurgia</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>204</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>56,00</t>
+          <t>68</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>NEUROLOGIA</t>
+          <t>Neurologia</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>260</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>33,14</t>
+          <t>37,1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>OBSTETRICIA E GINECOLOGIA</t>
+          <t>Obstetrícia e Ginecologia</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>386</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>454</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27,57</t>
+          <t>37,8</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>OFTALMOLOGIA</t>
+          <t>Oftalmologia</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>443</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>31,50</t>
+          <t>36,9</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ORTOPEDIA E TRAUMATOLOGIA</t>
+          <t>Ortopedia e Traumatologia</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>319</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>20,57</t>
+          <t>19,9</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>OTORRINOLARINGOLOGIA</t>
+          <t>Otorrinolaringologia</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>260</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>52,00</t>
+          <t>43,3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PATOLOGIA</t>
+          <t>Patologia</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>62</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14,25</t>
+          <t>15,5</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PATOLOGIA CLINICA/MEDICINA LABORATORIAL</t>
+          <t>Patologia Clínica e Medicina Laboratorial</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>2,5</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>PEDIATRIA</t>
+          <t>Pediatria</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>310</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13,19</t>
+          <t>17,2</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PSIQUIATRIA</t>
+          <t>Psiquiatria</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>344</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>552</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>43,00</t>
+          <t>36,8</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>RADIOLOGIA E DIAGNOSTICO POR IMAGEM</t>
+          <t>Radiologia e Diagnóstico por Imagem</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>232</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>21,43</t>
+          <t>19,3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>RADIOTERAPIA</t>
+          <t>Radioterapia</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -5685,6 +5510,619 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>PROGRAMAS ACESSO DIRETO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>CANDIDATOS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>VAGAS DISPONÍVEIS</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CONCORRÊNCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ANESTESIOLOGIA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>241</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>24,10</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CIRURGIA CARDIOVASCULAR</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>18,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CIRURGIA GERAL</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>483</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>40,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CLINICA MEDICA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>575</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>15,54</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DERMATOLOGIA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>244</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>48,80</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DERMATOLOGIA – COMPROMISSO SOCIAL</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>8,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GENETICA MEDICA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>INFECTOLOGIA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>7,80</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MEDICINA DE EMERGENCIA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>4,75</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MEDICINA DE FAMILIA E COMUNIDADE</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>10,07</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MEDICINA DO TRABALHO</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>7,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MEDICINA INTENSIVA</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5,71</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MEDICINA NUCLEAR</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>8,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MEDICINA PREVENTIVA E SOCIAL</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>NEUROCIRURGIA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>168</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>56,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>NEUROLOGIA</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>232</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>33,14</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>OBSTETRICIA E GINECOLOGIA</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>386</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>27,57</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>OFTALMOLOGIA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>31,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ORTOPEDIA E TRAUMATOLOGIA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>144</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>20,57</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>OTORRINOLARINGOLOGIA</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>260</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>52,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>PATOLOGIA</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>14,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PATOLOGIA CLINICA/MEDICINA LABORATORIAL</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PEDIATRIA</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>211</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>13,19</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PSIQUIATRIA</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>344</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>43,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>RADIOLOGIA E DIAGNOSTICO POR IMAGEM</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>21,43</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>RADIOTERAPIA</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5923,7 +6361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6294,7 +6732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8988,6 +9426,333 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Especialidade</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Inscritos</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Vagas</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Concorrência</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Anestesiologia</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>299</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>37.38</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cardiologia</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>5.71</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cirurgia Cardiovascular</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>15.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cirurgia da Mão</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cirurgia do Aparelho Digestivo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cirurgia Geral</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>498</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>38.31</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cirurgia Oncológica</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Cirurgia Pediátrica</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>7.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cirurgia Plástica</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cirurgia Torácica</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Cirurgia Vascular</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3.67</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Clínica Médica</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>663</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>22.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Dermatologia</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>350</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>58.33</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9243,7 +10008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -9326,441 +10091,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>PROGRAMA</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>VAGAS TOTAIS</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>INSCRITOS</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>CONCORRÊNCIA</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Anestesiologia</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>205</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Angiorradiologia e Cirurgia Endovascular</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0,33</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Cardiologia</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Cirurgia Cardiovascular</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Cirurgia Geral</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>196</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Cirurgia Vascular</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>4,33</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Clínica Médica</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>166</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>41,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Ginecologia e Obstetrícia</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>216</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>43,2</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Medicina de Família e Comunidade</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>7,67</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Medicina Intensiva Pediátrica</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Neonatologia</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1,33</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Neurocirurgia</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Oftalmologia</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>48,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Oncologia Clínica</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Ortopedia e Traumatologia</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>127</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>31,75</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Otorrinolaringologia</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Pediatria</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>157</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>39,25</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Urologia</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
🤖 Publica dados no site (04/11/2025 10:47)
</commit_message>
<xml_diff>
--- a/site/downloads/concorrencia_2026.xlsx
+++ b/site/downloads/concorrencia_2026.xlsx
@@ -13,17 +13,18 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SMS-Curitiba" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UFCSPA" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UEL" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNESP" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HIAE" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HOS BOS" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Santa Casa de Limeira" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SES-RJ" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UERJ" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNIFESP" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNICAMP" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instituto do Câncer do Ceará – " sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UFPA" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USP-SP" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNESP" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HIAE" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HOS BOS" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Santa Casa de Limeira" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SES-RJ" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UERJ" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNIFESP" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNICAMP" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instituto do Câncer do Ceará – " sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UFPA" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2512,6 +2513,91 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Especialidade</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Inscritos</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Vagas</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cand/Vaga</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Oftalmologia</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>705</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>88,12</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Otorrinolaringologia</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>235</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>78,33</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2943,7 +3029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4690,7 +4776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4888,619 +4974,6 @@
       <c r="C11" t="inlineStr">
         <is>
           <t>40,5</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>PROGRAMA</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL VAGAS</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL INSCRITOS</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>CONCORRÊNCIA GERAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Acupuntura</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>5,3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Anestesiologia</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>339</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>33,9</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Cirurgia Cardiovascular</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Cirurgia Geral</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>704</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Clínica Médica</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>905</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>17,4</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Dermatologia</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>370</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>46,3</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Genética Médica</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>17,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Infectologia</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Medicina de Emergência</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>5,8</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Medicina de Família e Comunidade</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>8,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Medicina de Tráfego</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0,7</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Medicina Esportiva</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>142</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>28,4</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Medicina Intensiva</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>5,6</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Medicina Preventiva e Social</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Neurocirurgia</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>204</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Neurologia</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>37,1</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Obstetrícia e Ginecologia</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>454</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>37,8</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Oftalmologia</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>443</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>36,9</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Ortopedia e Traumatologia</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>319</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>19,9</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Otorrinolaringologia</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>43,3</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Patologia</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>15,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Patologia Clínica e Medicina Laboratorial</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Pediatria</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>310</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>17,2</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Psiquiatria</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>552</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>36,8</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Radiologia e Diagnóstico por Imagem</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>232</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>19,3</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Radioterapia</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
     </row>
@@ -5526,139 +4999,139 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PROGRAMAS ACESSO DIRETO</t>
+          <t>PROGRAMA</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>CANDIDATOS</t>
+          <t>TOTAL VAGAS</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>VAGAS DISPONÍVEIS</t>
+          <t>TOTAL INSCRITOS</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CONCORRÊNCIA</t>
+          <t>CONCORRÊNCIA GERAL</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ANESTESIOLOGIA</t>
+          <t>Acupuntura</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>16</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>24,10</t>
+          <t>5,3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CIRURGIA CARDIOVASCULAR</t>
+          <t>Anestesiologia</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>339</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>18,00</t>
+          <t>33,9</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CIRURGIA GERAL</t>
+          <t>Cirurgia Cardiovascular</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>483</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>36</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>40,25</t>
+          <t>18</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CLINICA MEDICA</t>
+          <t>Cirurgia Geral</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>575</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>704</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>15,54</t>
+          <t>44</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DERMATOLOGIA</t>
+          <t>Clínica Médica</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>52</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>905</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>48,80</t>
+          <t>17,4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DERMATOLOGIA – COMPROMISSO SOCIAL</t>
+          <t>Dermatologia</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -5668,452 +5141,452 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>370</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>8,00</t>
+          <t>46,3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GENETICA MEDICA</t>
+          <t>Genética Médica</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10,00</t>
+          <t>17,5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>INFECTOLOGIA</t>
+          <t>Infectologia</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>42</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>7,80</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MEDICINA DE EMERGENCIA</t>
+          <t>Medicina de Emergência</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>64</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4,75</t>
+          <t>5,8</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MEDICINA DE FAMILIA E COMUNIDADE</t>
+          <t>Medicina de Família e Comunidade</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>34</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>10,07</t>
+          <t>8,5</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MEDICINA DO TRABALHO</t>
+          <t>Medicina de Tráfego</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>7,25</t>
+          <t>0,7</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MEDICINA INTENSIVA</t>
+          <t>Medicina Esportiva</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>142</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5,71</t>
+          <t>28,4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MEDICINA NUCLEAR</t>
+          <t>Medicina Intensiva</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>56</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>8,33</t>
+          <t>5,6</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MEDICINA PREVENTIVA E SOCIAL</t>
+          <t>Medicina Preventiva e Social</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1,25</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>NEUROCIRURGIA</t>
+          <t>Neurocirurgia</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>204</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>56,00</t>
+          <t>68</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>NEUROLOGIA</t>
+          <t>Neurologia</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>260</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>33,14</t>
+          <t>37,1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>OBSTETRICIA E GINECOLOGIA</t>
+          <t>Obstetrícia e Ginecologia</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>386</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>454</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27,57</t>
+          <t>37,8</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>OFTALMOLOGIA</t>
+          <t>Oftalmologia</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>443</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>31,50</t>
+          <t>36,9</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ORTOPEDIA E TRAUMATOLOGIA</t>
+          <t>Ortopedia e Traumatologia</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>319</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>20,57</t>
+          <t>19,9</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>OTORRINOLARINGOLOGIA</t>
+          <t>Otorrinolaringologia</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>260</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>52,00</t>
+          <t>43,3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PATOLOGIA</t>
+          <t>Patologia</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>62</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14,25</t>
+          <t>15,5</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PATOLOGIA CLINICA/MEDICINA LABORATORIAL</t>
+          <t>Patologia Clínica e Medicina Laboratorial</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2,00</t>
+          <t>2,5</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>PEDIATRIA</t>
+          <t>Pediatria</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>310</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13,19</t>
+          <t>17,2</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PSIQUIATRIA</t>
+          <t>Psiquiatria</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>344</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>552</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>43,00</t>
+          <t>36,8</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>RADIOLOGIA E DIAGNOSTICO POR IMAGEM</t>
+          <t>Radiologia e Diagnóstico por Imagem</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>232</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>21,43</t>
+          <t>19,3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>RADIOTERAPIA</t>
+          <t>Radioterapia</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -6123,6 +5596,619 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>PROGRAMAS ACESSO DIRETO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>CANDIDATOS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>VAGAS DISPONÍVEIS</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CONCORRÊNCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ANESTESIOLOGIA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>241</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>24,10</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CIRURGIA CARDIOVASCULAR</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>18,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CIRURGIA GERAL</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>483</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>40,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CLINICA MEDICA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>575</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>15,54</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DERMATOLOGIA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>244</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>48,80</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DERMATOLOGIA – COMPROMISSO SOCIAL</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>8,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GENETICA MEDICA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>INFECTOLOGIA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>7,80</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MEDICINA DE EMERGENCIA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>4,75</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MEDICINA DE FAMILIA E COMUNIDADE</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>10,07</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MEDICINA DO TRABALHO</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>7,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MEDICINA INTENSIVA</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5,71</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MEDICINA NUCLEAR</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>8,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MEDICINA PREVENTIVA E SOCIAL</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>NEUROCIRURGIA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>168</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>56,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>NEUROLOGIA</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>232</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>33,14</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>OBSTETRICIA E GINECOLOGIA</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>386</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>27,57</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>OFTALMOLOGIA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>31,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ORTOPEDIA E TRAUMATOLOGIA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>144</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>20,57</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>OTORRINOLARINGOLOGIA</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>260</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>52,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>PATOLOGIA</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>14,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PATOLOGIA CLINICA/MEDICINA LABORATORIAL</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PEDIATRIA</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>211</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>13,19</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PSIQUIATRIA</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>344</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>43,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>RADIOLOGIA E DIAGNOSTICO POR IMAGEM</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>21,43</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>RADIOTERAPIA</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6361,7 +6447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6732,7 +6818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -9426,6 +9512,217 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Especialidade</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Relação Candidato/Vaga</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Otorrinolaringologia</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>70,75</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Neurocirurgia</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>50,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Dermatologia</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>48,6</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cirurgia Geral</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>42,32</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Psiquiatria</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>40,61</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Obstetrícia e Ginecologia</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>38,38</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Oftalmologia</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>37,08</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Cirurgia Plástica</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>28,57</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Medicina do Trabalho</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ortopedia e Traumatologia</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>24,61</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Neurologia</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>24,18</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Medicina Esportiva</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>24,17</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Anestesiologia</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>20,91</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Clínica Médica</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>20,91</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Urologia</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>17,2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9747,7 +10044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -10006,89 +10303,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Especialidade</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Inscritos</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Vagas</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Cand/Vaga</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Oftalmologia</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>705</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>88,12</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Otorrinolaringologia</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>235</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>78,33</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
🤖 Publica dados no site (04/11/2025 17:22)
</commit_message>
<xml_diff>
--- a/site/downloads/concorrencia_2026.xlsx
+++ b/site/downloads/concorrencia_2026.xlsx
@@ -24434,17 +24434,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>DATA</t>
+          <t>PROGRAMA</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>HORÁRIO</t>
+          <t>VAGAS</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EVENTO</t>
+          <t>INSCRITOS</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -24456,17 +24456,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13/10/2025</t>
+          <t>Cancerologia Cirúrgica*</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>19h</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Gabarito ICC 2026</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>

<commit_message>
🤖 Publica dados no site (12/11/2025 10:12)
</commit_message>
<xml_diff>
--- a/site/downloads/concorrencia_2026.xlsx
+++ b/site/downloads/concorrencia_2026.xlsx
@@ -18,30 +18,31 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concorrência UEL 2026" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HONPAR" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hospital Pequeno Príncipe" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relação candidato vaga residênc" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USP-SP — Acesso Direto" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USP-SP — Pré-Requisito" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USP-SP — Pré-Requisito – Especi" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USP-SP — Áreas de Atuação e Ano" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concorrência Unesp 2026" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HIAE" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HOS BOS" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Santa Casa de Limeira" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concorrência SES-RJ 2026" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relação candidato vaga UERJ 202" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programas mais concorridos – UE" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relação Candidato Vaga Residênc1" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNICAMP — Concorrência AMP 2025" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PSU-ES SUL" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hospital Evangélico de Vila Vel" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instituto do Câncer do Ceará – " sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Secretaria Municipal de Saúde d" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UFPA" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Acesso Direto" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Pré-Requisito" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Área de Atuação" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Ano Adicional" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Quais as mais concorrid" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hospital Santa Rita" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relação candidato vaga residênc" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USP-SP — Acesso Direto" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USP-SP — Pré-Requisito" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USP-SP — Pré-Requisito – Especi" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USP-SP — Áreas de Atuação e Ano" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concorrência Unesp 2026" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HIAE" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HOS BOS" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Santa Casa de Limeira" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concorrência SES-RJ 2026" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relação candidato vaga UERJ 202" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Programas mais concorridos – UE" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relação Candidato Vaga Residênc1" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNICAMP — Concorrência AMP 2025" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PSU-ES SUL" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hospital Evangélico de Vila Vel" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instituto do Câncer do Ceará – " sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Secretaria Municipal de Saúde d" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UFPA" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Acesso Direto" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Pré-Requisito" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Área de Atuação" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Ano Adicional" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enare — Quais as mais concorrid" sheetId="36" state="visible" r:id="rId36"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -7396,6 +7397,399 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>PROGRAMA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>VAGAS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>INSCRITOS</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CONCORRÊNCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Anestesiologia</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>26,67</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cirurgia Geral</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>24,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Clínica Médica</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Infectologia</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Medicina Intensivo Adulto</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ortopedia e Traumatologia</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>16,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Pediatria</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Radiologia e Diagnóstico por Imagem</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>23,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cardiologia</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cirurgia Oncológica</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Cirurgia Vascular</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Coloproctologia</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ecocardiografia</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Gastroenterologia</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Neonatologia</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Oncologia Clínica</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7601,7 +7995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8302,7 +8696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8453,7 +8847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8890,7 +9284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -9833,7 +10227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -10732,7 +11126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -10985,91 +11379,6 @@
       <c r="D11" t="inlineStr">
         <is>
           <t>44,37</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Especialidade</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Inscritos</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Vagas</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Cand/Vaga</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Oftalmologia</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>705</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>88,12</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Otorrinolaringologia</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>235</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>78,33</t>
         </is>
       </c>
     </row>
@@ -11675,6 +11984,91 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Especialidade</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Inscritos</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Vagas</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cand/Vaga</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Oftalmologia</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>705</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>88,12</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Otorrinolaringologia</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>235</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>78,33</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12106,7 +12500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -13853,7 +14247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -15060,7 +15454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -15266,7 +15660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -18793,7 +19187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -25076,7 +25470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -25500,7 +25894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -25871,7 +26265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -26102,223 +26496,6 @@
       <c r="D10" t="inlineStr">
         <is>
           <t>19</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Programa</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Vagas</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Inscritos</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Concorrência</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Anestesiologia</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>149</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>74,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Cirurgia Geral</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>173</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>34,6</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Clínica Médica</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>227</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>22,7</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Coloproctologia</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>5,5</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Ginecologia e Obstetrícia</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>176</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Medicina de Família e Comunidade</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>342</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>17,1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Neonatologia</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1,33</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Ortopedia e Traumatologia</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>19,5</t>
         </is>
       </c>
     </row>
@@ -27672,6 +27849,223 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Vagas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Inscritos</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Concorrência</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Anestesiologia</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>74,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cirurgia Geral</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>173</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>34,6</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Clínica Médica</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>227</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>22,7</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Coloproctologia</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ginecologia e Obstetrícia</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>176</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Medicina de Família e Comunidade</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>342</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>17,1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Neonatologia</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1,33</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ortopedia e Traumatologia</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>19,5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28037,7 +28431,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -28760,7 +29154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -29307,7 +29701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -30448,7 +30842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -30995,7 +31389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>